<commit_message>
log before modifying excel sheet
</commit_message>
<xml_diff>
--- a/StudentWorkshop_SampleExcelSheet.xlsx
+++ b/StudentWorkshop_SampleExcelSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8700" tabRatio="224" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="224" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtübersicht" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="429">
   <si>
     <t>Werkstätten</t>
   </si>
@@ -1255,6 +1255,21 @@
   </si>
   <si>
     <t>Abed</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>Sch眉ler</t>
@@ -8227,7 +8242,7 @@
   <dimension ref="A1:S128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -8288,7 +8303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>412</v>
       </c>
@@ -8327,6 +8342,21 @@
       </c>
       <c r="M2">
         <v>4</v>
+      </c>
+      <c r="O2" t="s">
+        <v>413</v>
+      </c>
+      <c r="P2" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>415</v>
+      </c>
+      <c r="R2" t="s">
+        <v>416</v>
+      </c>
+      <c r="S2" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8775,7 +8805,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B15" t="s">
         <v>180</v>
@@ -9084,7 +9114,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B24" t="s">
         <v>203</v>
@@ -9959,7 +9989,7 @@
         <v>247</v>
       </c>
       <c r="B46" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="C46" t="s">
         <v>210</v>
@@ -9997,7 +10027,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="B47" t="s">
         <v>250</v>
@@ -10440,7 +10470,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="B60" t="s">
         <v>275</v>
@@ -10604,7 +10634,7 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B64" t="s">
         <v>284</v>
@@ -10708,7 +10738,7 @@
     </row>
     <row r="68" spans="1:13">
       <c r="A68" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="B68" t="s">
         <v>292</v>
@@ -10749,7 +10779,7 @@
     </row>
     <row r="69" spans="1:13">
       <c r="A69" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="B69" t="s">
         <v>294</v>
@@ -10831,7 +10861,7 @@
     </row>
     <row r="71" spans="1:13">
       <c r="A71" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="B71" t="s">
         <v>298</v>
@@ -12608,7 +12638,7 @@
     </row>
     <row r="118" spans="1:13">
       <c r="A118" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="B118" t="s">
         <v>393</v>
@@ -12947,7 +12977,7 @@
     </row>
     <row r="127" spans="1:13">
       <c r="A127" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="B127" t="s">
         <v>409</v>

</xml_diff>

<commit_message>
Fixed student repeating classes
- student with no preference are taking the class with the least participants
</commit_message>
<xml_diff>
--- a/StudentWorkshop_SampleExcelSheet.xlsx
+++ b/StudentWorkshop_SampleExcelSheet.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Wuensche" sheetId="2" r:id="rId2"/>
     <sheet name="Timetable" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Wuensche!$A$1:$S$128</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2814" uniqueCount="424">
   <si>
     <t>Werkstätten</t>
   </si>
@@ -1255,21 +1258,6 @@
   </si>
   <si>
     <t>Abed</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
   </si>
   <si>
     <t>Sch眉ler</t>
@@ -1993,148 +1981,148 @@
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="17">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="18">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="17">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="19">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
@@ -2499,7 +2487,7 @@
   <dimension ref="A1:BG130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -8242,7 +8230,9 @@
   <dimension ref="A1:S128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -8344,22 +8334,22 @@
         <v>4</v>
       </c>
       <c r="O2" t="s">
-        <v>413</v>
+        <v>33</v>
       </c>
       <c r="P2" t="s">
-        <v>414</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
-        <v>415</v>
+        <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>416</v>
+        <v>28</v>
       </c>
       <c r="S2" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -8399,8 +8389,23 @@
       <c r="M3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -8440,8 +8445,23 @@
       <c r="M4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -8463,8 +8483,23 @@
       <c r="I5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -8504,8 +8539,23 @@
       <c r="M6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -8545,8 +8595,23 @@
       <c r="M7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>47</v>
+      </c>
+      <c r="R7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -8586,8 +8651,23 @@
       <c r="M8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -8627,8 +8707,23 @@
       <c r="M9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -8668,8 +8763,23 @@
       <c r="M10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -8709,8 +8819,23 @@
       <c r="M11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -8750,8 +8875,23 @@
       <c r="M12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>153</v>
       </c>
@@ -8761,8 +8901,23 @@
       <c r="C13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="O13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>166</v>
       </c>
@@ -8802,10 +8957,25 @@
       <c r="M14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="O14" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" t="s">
+        <v>6</v>
+      </c>
+      <c r="S14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B15" t="s">
         <v>180</v>
@@ -8813,8 +8983,23 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -8824,8 +9009,23 @@
       <c r="C16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="O16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>47</v>
+      </c>
+      <c r="R16" t="s">
+        <v>8</v>
+      </c>
+      <c r="S16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>188</v>
       </c>
@@ -8865,8 +9065,23 @@
       <c r="M17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="O17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" t="s">
+        <v>6</v>
+      </c>
+      <c r="S17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -8906,8 +9121,23 @@
       <c r="M18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>29</v>
+      </c>
+      <c r="S18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>192</v>
       </c>
@@ -8947,8 +9177,23 @@
       <c r="M19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="O19" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>194</v>
       </c>
@@ -8988,8 +9233,23 @@
       <c r="M20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="O20" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>32</v>
+      </c>
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>196</v>
       </c>
@@ -9029,8 +9289,23 @@
       <c r="M21">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="O21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R21" t="s">
+        <v>6</v>
+      </c>
+      <c r="S21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -9070,8 +9345,23 @@
       <c r="M22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>5</v>
+      </c>
+      <c r="R22" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -9111,10 +9401,25 @@
       <c r="M23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="O23" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B24" t="s">
         <v>203</v>
@@ -9152,8 +9457,23 @@
       <c r="M24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="O24" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>6</v>
+      </c>
+      <c r="R24" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>204</v>
       </c>
@@ -9193,8 +9513,23 @@
       <c r="M25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="O25" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" t="s">
         <v>206</v>
       </c>
@@ -9234,8 +9569,23 @@
       <c r="M26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="O26" t="s">
+        <v>47</v>
+      </c>
+      <c r="P26" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>33</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -9275,8 +9625,23 @@
       <c r="M27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="O27" t="s">
+        <v>27</v>
+      </c>
+      <c r="P27" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>5</v>
+      </c>
+      <c r="R27" t="s">
+        <v>33</v>
+      </c>
+      <c r="S27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" t="s">
         <v>211</v>
       </c>
@@ -9316,8 +9681,23 @@
       <c r="M28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="O28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P28" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>6</v>
+      </c>
+      <c r="R28" t="s">
+        <v>8</v>
+      </c>
+      <c r="S28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" t="s">
         <v>213</v>
       </c>
@@ -9357,8 +9737,23 @@
       <c r="M29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="O29" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>5</v>
+      </c>
+      <c r="R29" t="s">
+        <v>33</v>
+      </c>
+      <c r="S29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -9398,8 +9793,23 @@
       <c r="M30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="O30" t="s">
+        <v>6</v>
+      </c>
+      <c r="P30" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>33</v>
+      </c>
+      <c r="R30" t="s">
+        <v>29</v>
+      </c>
+      <c r="S30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -9439,8 +9849,23 @@
       <c r="M31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="O31" t="s">
+        <v>8</v>
+      </c>
+      <c r="P31" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>27</v>
+      </c>
+      <c r="R31" t="s">
+        <v>33</v>
+      </c>
+      <c r="S31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" t="s">
         <v>219</v>
       </c>
@@ -9480,8 +9905,23 @@
       <c r="M32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="O32" t="s">
+        <v>8</v>
+      </c>
+      <c r="P32" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>5</v>
+      </c>
+      <c r="R32" t="s">
+        <v>6</v>
+      </c>
+      <c r="S32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>221</v>
       </c>
@@ -9521,8 +9961,23 @@
       <c r="M33">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="O33" t="s">
+        <v>5</v>
+      </c>
+      <c r="P33" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>8</v>
+      </c>
+      <c r="S33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>223</v>
       </c>
@@ -9562,8 +10017,23 @@
       <c r="M34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="O34" t="s">
+        <v>33</v>
+      </c>
+      <c r="P34" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>6</v>
+      </c>
+      <c r="R34" t="s">
+        <v>5</v>
+      </c>
+      <c r="S34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
         <v>225</v>
       </c>
@@ -9603,8 +10073,23 @@
       <c r="M35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="O35" t="s">
+        <v>29</v>
+      </c>
+      <c r="P35" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>6</v>
+      </c>
+      <c r="R35" t="s">
+        <v>5</v>
+      </c>
+      <c r="S35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>227</v>
       </c>
@@ -9644,8 +10129,23 @@
       <c r="M36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="O36" t="s">
+        <v>28</v>
+      </c>
+      <c r="P36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>47</v>
+      </c>
+      <c r="S36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>230</v>
       </c>
@@ -9685,8 +10185,23 @@
       <c r="M37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="O37" t="s">
+        <v>28</v>
+      </c>
+      <c r="P37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" t="s">
+        <v>47</v>
+      </c>
+      <c r="S37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>232</v>
       </c>
@@ -9726,8 +10241,23 @@
       <c r="M38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="O38" t="s">
+        <v>47</v>
+      </c>
+      <c r="P38" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>28</v>
+      </c>
+      <c r="R38" t="s">
+        <v>5</v>
+      </c>
+      <c r="S38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>234</v>
       </c>
@@ -9767,8 +10297,23 @@
       <c r="M39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="O39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>32</v>
+      </c>
+      <c r="R39" t="s">
+        <v>29</v>
+      </c>
+      <c r="S39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>236</v>
       </c>
@@ -9808,8 +10353,23 @@
       <c r="M40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="O40" t="s">
+        <v>6</v>
+      </c>
+      <c r="P40" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>32</v>
+      </c>
+      <c r="R40" t="s">
+        <v>1</v>
+      </c>
+      <c r="S40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -9849,8 +10409,23 @@
       <c r="M41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="O41" t="s">
+        <v>6</v>
+      </c>
+      <c r="P41" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>33</v>
+      </c>
+      <c r="R41" t="s">
+        <v>28</v>
+      </c>
+      <c r="S41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
         <v>239</v>
       </c>
@@ -9860,8 +10435,23 @@
       <c r="C42" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="O42" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>8</v>
+      </c>
+      <c r="R42" t="s">
+        <v>32</v>
+      </c>
+      <c r="S42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>241</v>
       </c>
@@ -9901,8 +10491,23 @@
       <c r="M43">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="O43" t="s">
+        <v>8</v>
+      </c>
+      <c r="P43" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>5</v>
+      </c>
+      <c r="R43" t="s">
+        <v>6</v>
+      </c>
+      <c r="S43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>243</v>
       </c>
@@ -9942,8 +10547,23 @@
       <c r="M44">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="O44" t="s">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>32</v>
+      </c>
+      <c r="R44" t="s">
+        <v>8</v>
+      </c>
+      <c r="S44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>245</v>
       </c>
@@ -9983,13 +10603,28 @@
       <c r="M45">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="O45" t="s">
+        <v>6</v>
+      </c>
+      <c r="P45" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>8</v>
+      </c>
+      <c r="R45" t="s">
+        <v>33</v>
+      </c>
+      <c r="S45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
         <v>247</v>
       </c>
       <c r="B46" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C46" t="s">
         <v>210</v>
@@ -10024,10 +10659,25 @@
       <c r="M46">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="O46" t="s">
+        <v>6</v>
+      </c>
+      <c r="P46" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>33</v>
+      </c>
+      <c r="R46" t="s">
+        <v>29</v>
+      </c>
+      <c r="S46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B47" t="s">
         <v>250</v>
@@ -10035,8 +10685,23 @@
       <c r="C47" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="O47" t="s">
+        <v>32</v>
+      </c>
+      <c r="P47" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R47" t="s">
+        <v>28</v>
+      </c>
+      <c r="S47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>251</v>
       </c>
@@ -10076,8 +10741,23 @@
       <c r="M48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="O48" t="s">
+        <v>29</v>
+      </c>
+      <c r="P48" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>33</v>
+      </c>
+      <c r="R48" t="s">
+        <v>5</v>
+      </c>
+      <c r="S48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>253</v>
       </c>
@@ -10117,8 +10797,23 @@
       <c r="M49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="O49" t="s">
+        <v>47</v>
+      </c>
+      <c r="P49" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>28</v>
+      </c>
+      <c r="R49" t="s">
+        <v>32</v>
+      </c>
+      <c r="S49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>255</v>
       </c>
@@ -10158,8 +10853,23 @@
       <c r="M50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="O50" t="s">
+        <v>33</v>
+      </c>
+      <c r="P50" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>6</v>
+      </c>
+      <c r="R50" t="s">
+        <v>5</v>
+      </c>
+      <c r="S50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" t="s">
         <v>257</v>
       </c>
@@ -10199,8 +10909,23 @@
       <c r="M51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="O51" t="s">
+        <v>33</v>
+      </c>
+      <c r="P51" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>27</v>
+      </c>
+      <c r="R51" t="s">
+        <v>29</v>
+      </c>
+      <c r="S51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>259</v>
       </c>
@@ -10240,8 +10965,23 @@
       <c r="M52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="O52" t="s">
+        <v>28</v>
+      </c>
+      <c r="P52" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>47</v>
+      </c>
+      <c r="R52" t="s">
+        <v>5</v>
+      </c>
+      <c r="S52" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>261</v>
       </c>
@@ -10281,8 +11021,23 @@
       <c r="M53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="O53" t="s">
+        <v>6</v>
+      </c>
+      <c r="P53" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>8</v>
+      </c>
+      <c r="R53" t="s">
+        <v>33</v>
+      </c>
+      <c r="S53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>264</v>
       </c>
@@ -10292,8 +11047,23 @@
       <c r="C54" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="O54" t="s">
+        <v>1</v>
+      </c>
+      <c r="P54" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>47</v>
+      </c>
+      <c r="R54" t="s">
+        <v>5</v>
+      </c>
+      <c r="S54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>264</v>
       </c>
@@ -10333,8 +11103,23 @@
       <c r="M55">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="O55" t="s">
+        <v>27</v>
+      </c>
+      <c r="P55" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>29</v>
+      </c>
+      <c r="R55" t="s">
+        <v>33</v>
+      </c>
+      <c r="S55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>267</v>
       </c>
@@ -10374,8 +11159,23 @@
       <c r="M56">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="O56" t="s">
+        <v>5</v>
+      </c>
+      <c r="P56" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>8</v>
+      </c>
+      <c r="R56" t="s">
+        <v>1</v>
+      </c>
+      <c r="S56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>269</v>
       </c>
@@ -10385,8 +11185,23 @@
       <c r="C57" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="O57" t="s">
+        <v>32</v>
+      </c>
+      <c r="P57" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>8</v>
+      </c>
+      <c r="R57" t="s">
+        <v>47</v>
+      </c>
+      <c r="S57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>271</v>
       </c>
@@ -10426,8 +11241,23 @@
       <c r="M58">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="O58" t="s">
+        <v>27</v>
+      </c>
+      <c r="P58" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>29</v>
+      </c>
+      <c r="R58" t="s">
+        <v>33</v>
+      </c>
+      <c r="S58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>273</v>
       </c>
@@ -10467,10 +11297,25 @@
       <c r="M59">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="O59" t="s">
+        <v>29</v>
+      </c>
+      <c r="P59" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>6</v>
+      </c>
+      <c r="R59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B60" t="s">
         <v>275</v>
@@ -10508,8 +11353,23 @@
       <c r="M60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="O60" t="s">
+        <v>29</v>
+      </c>
+      <c r="P60" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>28</v>
+      </c>
+      <c r="R60" t="s">
+        <v>33</v>
+      </c>
+      <c r="S60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>276</v>
       </c>
@@ -10549,8 +11409,23 @@
       <c r="M61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="O61" t="s">
+        <v>29</v>
+      </c>
+      <c r="P61" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>28</v>
+      </c>
+      <c r="R61" t="s">
+        <v>33</v>
+      </c>
+      <c r="S61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" t="s">
         <v>278</v>
       </c>
@@ -10590,8 +11465,23 @@
       <c r="M62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="O62" t="s">
+        <v>28</v>
+      </c>
+      <c r="P62" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>1</v>
+      </c>
+      <c r="R62" t="s">
+        <v>5</v>
+      </c>
+      <c r="S62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" t="s">
         <v>281</v>
       </c>
@@ -10631,10 +11521,25 @@
       <c r="M63">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="O63" t="s">
+        <v>33</v>
+      </c>
+      <c r="P63" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>1</v>
+      </c>
+      <c r="R63" t="s">
+        <v>47</v>
+      </c>
+      <c r="S63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B64" t="s">
         <v>284</v>
@@ -10672,8 +11577,23 @@
       <c r="M64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="O64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P64" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>6</v>
+      </c>
+      <c r="R64" t="s">
+        <v>5</v>
+      </c>
+      <c r="S64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" t="s">
         <v>285</v>
       </c>
@@ -10683,8 +11603,23 @@
       <c r="C65" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="O65" t="s">
+        <v>1</v>
+      </c>
+      <c r="P65" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>32</v>
+      </c>
+      <c r="R65" t="s">
+        <v>6</v>
+      </c>
+      <c r="S65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" t="s">
         <v>287</v>
       </c>
@@ -10694,8 +11629,23 @@
       <c r="C66" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="O66" t="s">
+        <v>32</v>
+      </c>
+      <c r="P66" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>1</v>
+      </c>
+      <c r="R66" t="s">
+        <v>28</v>
+      </c>
+      <c r="S66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" t="s">
         <v>289</v>
       </c>
@@ -10735,10 +11685,25 @@
       <c r="M67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="O67" t="s">
+        <v>33</v>
+      </c>
+      <c r="P67" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>29</v>
+      </c>
+      <c r="R67" t="s">
+        <v>32</v>
+      </c>
+      <c r="S67" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B68" t="s">
         <v>292</v>
@@ -10776,10 +11741,25 @@
       <c r="M68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="O68" t="s">
+        <v>27</v>
+      </c>
+      <c r="P68" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>28</v>
+      </c>
+      <c r="R68" t="s">
+        <v>33</v>
+      </c>
+      <c r="S68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B69" t="s">
         <v>294</v>
@@ -10817,8 +11797,23 @@
       <c r="M69">
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="O69" t="s">
+        <v>1</v>
+      </c>
+      <c r="P69" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>29</v>
+      </c>
+      <c r="R69" t="s">
+        <v>8</v>
+      </c>
+      <c r="S69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" t="s">
         <v>295</v>
       </c>
@@ -10858,10 +11853,25 @@
       <c r="M70">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="O70" t="s">
+        <v>6</v>
+      </c>
+      <c r="P70" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>29</v>
+      </c>
+      <c r="R70" t="s">
+        <v>8</v>
+      </c>
+      <c r="S70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
       <c r="A71" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B71" t="s">
         <v>298</v>
@@ -10899,8 +11909,23 @@
       <c r="M71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="O71" t="s">
+        <v>28</v>
+      </c>
+      <c r="P71" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>29</v>
+      </c>
+      <c r="R71" t="s">
+        <v>32</v>
+      </c>
+      <c r="S71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
       <c r="A72" t="s">
         <v>299</v>
       </c>
@@ -10940,8 +11965,23 @@
       <c r="M72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="O72" t="s">
+        <v>27</v>
+      </c>
+      <c r="P72" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>6</v>
+      </c>
+      <c r="R72" t="s">
+        <v>47</v>
+      </c>
+      <c r="S72" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
       <c r="A73" t="s">
         <v>301</v>
       </c>
@@ -10981,8 +12021,23 @@
       <c r="M73">
         <v>7</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="O73" t="s">
+        <v>6</v>
+      </c>
+      <c r="P73" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>8</v>
+      </c>
+      <c r="R73" t="s">
+        <v>33</v>
+      </c>
+      <c r="S73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
       <c r="A74" t="s">
         <v>303</v>
       </c>
@@ -11022,8 +12077,23 @@
       <c r="M74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="O74" t="s">
+        <v>29</v>
+      </c>
+      <c r="P74" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>47</v>
+      </c>
+      <c r="R74" t="s">
+        <v>27</v>
+      </c>
+      <c r="S74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
       <c r="A75" t="s">
         <v>305</v>
       </c>
@@ -11063,8 +12133,23 @@
       <c r="M75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
+      <c r="O75" t="s">
+        <v>29</v>
+      </c>
+      <c r="P75" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>27</v>
+      </c>
+      <c r="R75" t="s">
+        <v>6</v>
+      </c>
+      <c r="S75" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
       <c r="A76" t="s">
         <v>307</v>
       </c>
@@ -11074,8 +12159,23 @@
       <c r="C76" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="O76" t="s">
+        <v>8</v>
+      </c>
+      <c r="P76" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>32</v>
+      </c>
+      <c r="R76" t="s">
+        <v>29</v>
+      </c>
+      <c r="S76" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" t="s">
         <v>309</v>
       </c>
@@ -11115,8 +12215,23 @@
       <c r="M77">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="O77" t="s">
+        <v>27</v>
+      </c>
+      <c r="P77" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>1</v>
+      </c>
+      <c r="R77" t="s">
+        <v>33</v>
+      </c>
+      <c r="S77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" t="s">
         <v>311</v>
       </c>
@@ -11156,8 +12271,23 @@
       <c r="M78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="O78" t="s">
+        <v>27</v>
+      </c>
+      <c r="P78" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>1</v>
+      </c>
+      <c r="R78" t="s">
+        <v>32</v>
+      </c>
+      <c r="S78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
       <c r="A79" t="s">
         <v>313</v>
       </c>
@@ -11197,8 +12327,23 @@
       <c r="M79">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="O79" t="s">
+        <v>8</v>
+      </c>
+      <c r="P79" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>5</v>
+      </c>
+      <c r="R79" t="s">
+        <v>33</v>
+      </c>
+      <c r="S79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" t="s">
         <v>316</v>
       </c>
@@ -11208,8 +12353,23 @@
       <c r="C80" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="O80" t="s">
+        <v>1</v>
+      </c>
+      <c r="P80" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>47</v>
+      </c>
+      <c r="R80" t="s">
+        <v>8</v>
+      </c>
+      <c r="S80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" t="s">
         <v>318</v>
       </c>
@@ -11219,8 +12379,23 @@
       <c r="C81" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="O81" t="s">
+        <v>32</v>
+      </c>
+      <c r="P81" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>1</v>
+      </c>
+      <c r="R81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" t="s">
         <v>319</v>
       </c>
@@ -11260,8 +12435,23 @@
       <c r="M82">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="O82" t="s">
+        <v>33</v>
+      </c>
+      <c r="P82" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>8</v>
+      </c>
+      <c r="R82" t="s">
+        <v>29</v>
+      </c>
+      <c r="S82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" t="s">
         <v>321</v>
       </c>
@@ -11301,8 +12491,23 @@
       <c r="M83">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="O83" t="s">
+        <v>33</v>
+      </c>
+      <c r="P83" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>5</v>
+      </c>
+      <c r="R83" t="s">
+        <v>29</v>
+      </c>
+      <c r="S83" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" t="s">
         <v>323</v>
       </c>
@@ -11342,8 +12547,23 @@
       <c r="M84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="O84" t="s">
+        <v>1</v>
+      </c>
+      <c r="P84" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>8</v>
+      </c>
+      <c r="R84" t="s">
+        <v>29</v>
+      </c>
+      <c r="S84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" t="s">
         <v>325</v>
       </c>
@@ -11383,8 +12603,23 @@
       <c r="M85">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="O85" t="s">
+        <v>33</v>
+      </c>
+      <c r="P85" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>5</v>
+      </c>
+      <c r="R85" t="s">
+        <v>29</v>
+      </c>
+      <c r="S85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" t="s">
         <v>327</v>
       </c>
@@ -11424,8 +12659,23 @@
       <c r="M86">
         <v>3</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="O86" t="s">
+        <v>47</v>
+      </c>
+      <c r="P86" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>28</v>
+      </c>
+      <c r="R86" t="s">
+        <v>6</v>
+      </c>
+      <c r="S86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" t="s">
         <v>329</v>
       </c>
@@ -11465,8 +12715,23 @@
       <c r="M87">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="O87" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>6</v>
+      </c>
+      <c r="R87" t="s">
+        <v>28</v>
+      </c>
+      <c r="S87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" t="s">
         <v>331</v>
       </c>
@@ -11506,8 +12771,23 @@
       <c r="M88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="O88" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>5</v>
+      </c>
+      <c r="R88" t="s">
+        <v>6</v>
+      </c>
+      <c r="S88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" t="s">
         <v>333</v>
       </c>
@@ -11547,8 +12827,23 @@
       <c r="M89">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="O89" t="s">
+        <v>33</v>
+      </c>
+      <c r="P89" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>28</v>
+      </c>
+      <c r="R89" t="s">
+        <v>29</v>
+      </c>
+      <c r="S89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" t="s">
         <v>334</v>
       </c>
@@ -11588,8 +12883,23 @@
       <c r="M90">
         <v>7</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="O90" t="s">
+        <v>27</v>
+      </c>
+      <c r="P90" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>6</v>
+      </c>
+      <c r="R90" t="s">
+        <v>29</v>
+      </c>
+      <c r="S90" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" t="s">
         <v>336</v>
       </c>
@@ -11629,8 +12939,23 @@
       <c r="M91">
         <v>8</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="O91" t="s">
+        <v>33</v>
+      </c>
+      <c r="P91" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>5</v>
+      </c>
+      <c r="R91" t="s">
+        <v>6</v>
+      </c>
+      <c r="S91" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" t="s">
         <v>338</v>
       </c>
@@ -11670,8 +12995,23 @@
       <c r="M92">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="O92" t="s">
+        <v>47</v>
+      </c>
+      <c r="P92" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>27</v>
+      </c>
+      <c r="R92" t="s">
+        <v>33</v>
+      </c>
+      <c r="S92" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" t="s">
         <v>341</v>
       </c>
@@ -11711,8 +13051,23 @@
       <c r="M93">
         <v>10</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="O93" t="s">
+        <v>32</v>
+      </c>
+      <c r="P93" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>47</v>
+      </c>
+      <c r="R93" t="s">
+        <v>8</v>
+      </c>
+      <c r="S93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" t="s">
         <v>343</v>
       </c>
@@ -11752,8 +13107,23 @@
       <c r="M94">
         <v>7</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
+      <c r="O94" t="s">
+        <v>47</v>
+      </c>
+      <c r="P94" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>27</v>
+      </c>
+      <c r="R94" t="s">
+        <v>29</v>
+      </c>
+      <c r="S94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" t="s">
         <v>345</v>
       </c>
@@ -11763,8 +13133,23 @@
       <c r="C95" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="96" spans="1:13">
+      <c r="O95" t="s">
+        <v>8</v>
+      </c>
+      <c r="P95" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>32</v>
+      </c>
+      <c r="R95" t="s">
+        <v>47</v>
+      </c>
+      <c r="S95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19">
       <c r="A96" t="s">
         <v>347</v>
       </c>
@@ -11804,8 +13189,23 @@
       <c r="M96">
         <v>6</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
+      <c r="O96" t="s">
+        <v>27</v>
+      </c>
+      <c r="P96" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>1</v>
+      </c>
+      <c r="R96" t="s">
+        <v>32</v>
+      </c>
+      <c r="S96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19">
       <c r="A97" t="s">
         <v>349</v>
       </c>
@@ -11845,8 +13245,23 @@
       <c r="M97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:13">
+      <c r="O97" t="s">
+        <v>47</v>
+      </c>
+      <c r="P97" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>28</v>
+      </c>
+      <c r="R97" t="s">
+        <v>6</v>
+      </c>
+      <c r="S97" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19">
       <c r="A98" t="s">
         <v>351</v>
       </c>
@@ -11886,8 +13301,23 @@
       <c r="M98">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
+      <c r="O98" t="s">
+        <v>47</v>
+      </c>
+      <c r="P98" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>1</v>
+      </c>
+      <c r="R98" t="s">
+        <v>28</v>
+      </c>
+      <c r="S98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19">
       <c r="A99" t="s">
         <v>353</v>
       </c>
@@ -11927,8 +13357,23 @@
       <c r="M99">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:13">
+      <c r="O99" t="s">
+        <v>47</v>
+      </c>
+      <c r="P99" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>1</v>
+      </c>
+      <c r="R99" t="s">
+        <v>28</v>
+      </c>
+      <c r="S99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19">
       <c r="A100" t="s">
         <v>355</v>
       </c>
@@ -11968,8 +13413,23 @@
       <c r="M100">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:13">
+      <c r="O100" t="s">
+        <v>47</v>
+      </c>
+      <c r="P100" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>32</v>
+      </c>
+      <c r="R100" t="s">
+        <v>28</v>
+      </c>
+      <c r="S100" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19">
       <c r="A101" t="s">
         <v>357</v>
       </c>
@@ -12009,8 +13469,23 @@
       <c r="M101">
         <v>2</v>
       </c>
-    </row>
-    <row r="102" spans="1:13">
+      <c r="O101" t="s">
+        <v>27</v>
+      </c>
+      <c r="P101" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>5</v>
+      </c>
+      <c r="R101" t="s">
+        <v>32</v>
+      </c>
+      <c r="S101" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19">
       <c r="A102" t="s">
         <v>359</v>
       </c>
@@ -12050,8 +13525,23 @@
       <c r="M102">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:13">
+      <c r="O102" t="s">
+        <v>47</v>
+      </c>
+      <c r="P102" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>32</v>
+      </c>
+      <c r="R102" t="s">
+        <v>28</v>
+      </c>
+      <c r="S102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19">
       <c r="A103" t="s">
         <v>361</v>
       </c>
@@ -12091,8 +13581,23 @@
       <c r="M103">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:13">
+      <c r="O103" t="s">
+        <v>1</v>
+      </c>
+      <c r="P103" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q103" t="s">
+        <v>32</v>
+      </c>
+      <c r="R103" t="s">
+        <v>28</v>
+      </c>
+      <c r="S103" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19">
       <c r="A104" t="s">
         <v>363</v>
       </c>
@@ -12132,8 +13637,23 @@
       <c r="M104">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:13">
+      <c r="O104" t="s">
+        <v>5</v>
+      </c>
+      <c r="P104" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>6</v>
+      </c>
+      <c r="R104" t="s">
+        <v>47</v>
+      </c>
+      <c r="S104" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19">
       <c r="A105" t="s">
         <v>366</v>
       </c>
@@ -12173,8 +13693,23 @@
       <c r="M105">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:13">
+      <c r="O105" t="s">
+        <v>29</v>
+      </c>
+      <c r="P105" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>33</v>
+      </c>
+      <c r="R105" t="s">
+        <v>8</v>
+      </c>
+      <c r="S105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19">
       <c r="A106" t="s">
         <v>368</v>
       </c>
@@ -12214,8 +13749,23 @@
       <c r="M106">
         <v>2</v>
       </c>
-    </row>
-    <row r="107" spans="1:13">
+      <c r="O106" t="s">
+        <v>6</v>
+      </c>
+      <c r="P106" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>33</v>
+      </c>
+      <c r="R106" t="s">
+        <v>8</v>
+      </c>
+      <c r="S106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19">
       <c r="A107" t="s">
         <v>370</v>
       </c>
@@ -12255,8 +13805,23 @@
       <c r="M107">
         <v>2</v>
       </c>
-    </row>
-    <row r="108" spans="1:13">
+      <c r="O107" t="s">
+        <v>5</v>
+      </c>
+      <c r="P107" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>29</v>
+      </c>
+      <c r="R107" t="s">
+        <v>6</v>
+      </c>
+      <c r="S107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19">
       <c r="A108" t="s">
         <v>372</v>
       </c>
@@ -12296,8 +13861,23 @@
       <c r="M108">
         <v>10</v>
       </c>
-    </row>
-    <row r="109" spans="1:13">
+      <c r="O108" t="s">
+        <v>5</v>
+      </c>
+      <c r="P108" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>33</v>
+      </c>
+      <c r="R108" t="s">
+        <v>8</v>
+      </c>
+      <c r="S108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19">
       <c r="A109" t="s">
         <v>374</v>
       </c>
@@ -12337,8 +13917,23 @@
       <c r="M109">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:13">
+      <c r="O109" t="s">
+        <v>27</v>
+      </c>
+      <c r="P109" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>6</v>
+      </c>
+      <c r="R109" t="s">
+        <v>8</v>
+      </c>
+      <c r="S109" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19">
       <c r="A110" t="s">
         <v>376</v>
       </c>
@@ -12378,8 +13973,23 @@
       <c r="M110">
         <v>10</v>
       </c>
-    </row>
-    <row r="111" spans="1:13">
+      <c r="O110" t="s">
+        <v>33</v>
+      </c>
+      <c r="P110" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>5</v>
+      </c>
+      <c r="R110" t="s">
+        <v>27</v>
+      </c>
+      <c r="S110" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19">
       <c r="A111" t="s">
         <v>378</v>
       </c>
@@ -12419,8 +14029,23 @@
       <c r="M111">
         <v>8</v>
       </c>
-    </row>
-    <row r="112" spans="1:13">
+      <c r="O111" t="s">
+        <v>27</v>
+      </c>
+      <c r="P111" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>29</v>
+      </c>
+      <c r="R111" t="s">
+        <v>1</v>
+      </c>
+      <c r="S111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19">
       <c r="A112" t="s">
         <v>380</v>
       </c>
@@ -12460,8 +14085,23 @@
       <c r="M112">
         <v>8</v>
       </c>
-    </row>
-    <row r="113" spans="1:13">
+      <c r="O112" t="s">
+        <v>27</v>
+      </c>
+      <c r="P112" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q112" t="s">
+        <v>33</v>
+      </c>
+      <c r="R112" t="s">
+        <v>8</v>
+      </c>
+      <c r="S112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19">
       <c r="A113" t="s">
         <v>381</v>
       </c>
@@ -12501,8 +14141,23 @@
       <c r="M113">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="O113" t="s">
+        <v>33</v>
+      </c>
+      <c r="P113" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>32</v>
+      </c>
+      <c r="R113" t="s">
+        <v>5</v>
+      </c>
+      <c r="S113" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19">
       <c r="A114" t="s">
         <v>383</v>
       </c>
@@ -12512,8 +14167,23 @@
       <c r="C114" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="115" spans="1:13">
+      <c r="O114" t="s">
+        <v>1</v>
+      </c>
+      <c r="P114" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q114" t="s">
+        <v>47</v>
+      </c>
+      <c r="R114" t="s">
+        <v>32</v>
+      </c>
+      <c r="S114" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19">
       <c r="A115" t="s">
         <v>385</v>
       </c>
@@ -12553,8 +14223,23 @@
       <c r="M115">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:13">
+      <c r="O115" t="s">
+        <v>27</v>
+      </c>
+      <c r="P115" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>33</v>
+      </c>
+      <c r="R115" t="s">
+        <v>5</v>
+      </c>
+      <c r="S115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19">
       <c r="A116" t="s">
         <v>387</v>
       </c>
@@ -12594,8 +14279,23 @@
       <c r="M116">
         <v>10</v>
       </c>
-    </row>
-    <row r="117" spans="1:13">
+      <c r="O116" t="s">
+        <v>6</v>
+      </c>
+      <c r="P116" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>33</v>
+      </c>
+      <c r="R116" t="s">
+        <v>27</v>
+      </c>
+      <c r="S116" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19">
       <c r="A117" t="s">
         <v>390</v>
       </c>
@@ -12635,10 +14335,25 @@
       <c r="M117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:13">
+      <c r="O117" t="s">
+        <v>28</v>
+      </c>
+      <c r="P117" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>6</v>
+      </c>
+      <c r="R117" t="s">
+        <v>47</v>
+      </c>
+      <c r="S117" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19">
       <c r="A118" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B118" t="s">
         <v>393</v>
@@ -12676,8 +14391,23 @@
       <c r="M118">
         <v>10</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="O118" t="s">
+        <v>6</v>
+      </c>
+      <c r="P118" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>33</v>
+      </c>
+      <c r="R118" t="s">
+        <v>27</v>
+      </c>
+      <c r="S118" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19">
       <c r="A119" t="s">
         <v>394</v>
       </c>
@@ -12687,8 +14417,23 @@
       <c r="C119" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="120" spans="1:13">
+      <c r="O119" t="s">
+        <v>32</v>
+      </c>
+      <c r="P119" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>8</v>
+      </c>
+      <c r="R119" t="s">
+        <v>1</v>
+      </c>
+      <c r="S119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19">
       <c r="A120" t="s">
         <v>396</v>
       </c>
@@ -12728,8 +14473,23 @@
       <c r="M120">
         <v>6</v>
       </c>
-    </row>
-    <row r="121" spans="1:13">
+      <c r="O120" t="s">
+        <v>6</v>
+      </c>
+      <c r="P120" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>29</v>
+      </c>
+      <c r="R120" t="s">
+        <v>5</v>
+      </c>
+      <c r="S120" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19">
       <c r="A121" t="s">
         <v>398</v>
       </c>
@@ -12769,8 +14529,23 @@
       <c r="M121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:13">
+      <c r="O121" t="s">
+        <v>28</v>
+      </c>
+      <c r="P121" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>47</v>
+      </c>
+      <c r="R121" t="s">
+        <v>27</v>
+      </c>
+      <c r="S121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19">
       <c r="A122" t="s">
         <v>276</v>
       </c>
@@ -12810,8 +14585,23 @@
       <c r="M122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:13">
+      <c r="O122" t="s">
+        <v>28</v>
+      </c>
+      <c r="P122" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>33</v>
+      </c>
+      <c r="R122" t="s">
+        <v>5</v>
+      </c>
+      <c r="S122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19">
       <c r="A123" t="s">
         <v>401</v>
       </c>
@@ -12851,8 +14641,23 @@
       <c r="M123">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:13">
+      <c r="O123" t="s">
+        <v>1</v>
+      </c>
+      <c r="P123" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>27</v>
+      </c>
+      <c r="R123" t="s">
+        <v>29</v>
+      </c>
+      <c r="S123" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19">
       <c r="A124" t="s">
         <v>349</v>
       </c>
@@ -12892,8 +14697,23 @@
       <c r="M124">
         <v>8</v>
       </c>
-    </row>
-    <row r="125" spans="1:13">
+      <c r="O124" t="s">
+        <v>27</v>
+      </c>
+      <c r="P124" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q124" t="s">
+        <v>1</v>
+      </c>
+      <c r="R124" t="s">
+        <v>32</v>
+      </c>
+      <c r="S124" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19">
       <c r="A125" t="s">
         <v>404</v>
       </c>
@@ -12933,8 +14753,23 @@
       <c r="M125">
         <v>3</v>
       </c>
-    </row>
-    <row r="126" spans="1:13">
+      <c r="O125" t="s">
+        <v>29</v>
+      </c>
+      <c r="P125" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>28</v>
+      </c>
+      <c r="R125" t="s">
+        <v>33</v>
+      </c>
+      <c r="S125" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19">
       <c r="A126" t="s">
         <v>406</v>
       </c>
@@ -12974,10 +14809,25 @@
       <c r="M126">
         <v>7</v>
       </c>
-    </row>
-    <row r="127" spans="1:13">
+      <c r="O126" t="s">
+        <v>47</v>
+      </c>
+      <c r="P126" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>27</v>
+      </c>
+      <c r="R126" t="s">
+        <v>5</v>
+      </c>
+      <c r="S126" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19">
       <c r="A127" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B127" t="s">
         <v>409</v>
@@ -13015,8 +14865,23 @@
       <c r="M127">
         <v>3</v>
       </c>
-    </row>
-    <row r="128" spans="1:13">
+      <c r="O127" t="s">
+        <v>1</v>
+      </c>
+      <c r="P127" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>28</v>
+      </c>
+      <c r="R127" t="s">
+        <v>8</v>
+      </c>
+      <c r="S127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19">
       <c r="A128" t="s">
         <v>410</v>
       </c>
@@ -13056,8 +14921,26 @@
       <c r="M128">
         <v>1</v>
       </c>
+      <c r="O128" t="s">
+        <v>28</v>
+      </c>
+      <c r="P128" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q128" t="s">
+        <v>47</v>
+      </c>
+      <c r="R128" t="s">
+        <v>6</v>
+      </c>
+      <c r="S128" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S128">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -13146,7 +15029,7 @@
       <c r="AW1" s="2"/>
       <c r="AX1" s="12"/>
     </row>
-    <row r="2" ht="15.15" spans="1:50">
+    <row r="2" ht="15.15" customHeight="1" spans="1:50">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
inconsistent class list fixed
-however the logic can be optimized as some students cannot be placed within the maximum 13 range with the current code
</commit_message>
<xml_diff>
--- a/StudentWorkshop_SampleExcelSheet.xlsx
+++ b/StudentWorkshop_SampleExcelSheet.xlsx
@@ -10488,7 +10488,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.888888888888889" defaultRowHeight="14.4"/>
@@ -10829,6 +10829,31 @@
       <c r="I5" t="n">
         <v>2</v>
       </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Handel</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -11350,6 +11375,31 @@
           <t>w/8a</t>
         </is>
       </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -11439,6 +11489,31 @@
           <t>m/8a</t>
         </is>
       </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Handel</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -11456,6 +11531,31 @@
           <t>m/8a</t>
         </is>
       </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Handel</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -13273,6 +13373,31 @@
           <t>m/8b</t>
         </is>
       </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>Büro</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -13578,6 +13703,31 @@
           <t>m/8b</t>
         </is>
       </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -14027,6 +14177,31 @@
           <t>m/8c</t>
         </is>
       </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Elektro</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -14188,6 +14363,31 @@
           <t>m/8c</t>
         </is>
       </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Handel</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Medien/IT</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -14709,6 +14909,31 @@
           <t>w/8c</t>
         </is>
       </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Medien/IT</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>Büro</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -14726,6 +14951,31 @@
           <t>m/8c</t>
         </is>
       </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -15391,6 +15641,31 @@
           <t>w/8c</t>
         </is>
       </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Elektro</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -15624,6 +15899,31 @@
           <t>m/8d</t>
         </is>
       </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>Büro</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -15641,6 +15941,31 @@
           <t>m/8d</t>
         </is>
       </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -16594,6 +16919,31 @@
           <t>w/8d</t>
         </is>
       </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Handel</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -17907,6 +18257,31 @@
           <t>m/8e</t>
         </is>
       </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>Medien/IT</t>
+        </is>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -18210,6 +18585,31 @@
       <c r="C119" t="inlineStr">
         <is>
           <t>w/8e</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>Holz</t>
+        </is>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>Druck</t>
+        </is>
+      </c>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>Handel</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed case where student can't fit in any class
Student who cannot fit into any class (previously must go to a class that exceed the maximum) now will re-arrange their class so they can have 5 classes without making one session exceed its maximum size
</commit_message>
<xml_diff>
--- a/StudentWorkshop_SampleExcelSheet.xlsx
+++ b/StudentWorkshop_SampleExcelSheet.xlsx
@@ -10486,9 +10486,9 @@
   <dimension ref="A1:S129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomLeft" activeCell="U74" sqref="U74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.888888888888889" defaultRowHeight="14.4"/>
@@ -15643,22 +15643,22 @@
       </c>
       <c r="O76" t="inlineStr">
         <is>
+          <t>Ges./Soz.</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Textil</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>Körper</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
           <t>Druck</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>Textil</t>
-        </is>
-      </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>Körper</t>
-        </is>
-      </c>
-      <c r="R76" t="inlineStr">
-        <is>
-          <t>Elektro</t>
         </is>
       </c>
       <c r="S76" t="inlineStr">
@@ -15901,7 +15901,7 @@
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Ges./Soz.</t>
+          <t>Körper</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">

</xml_diff>